<commit_message>
v0.5 Gerbers sent for manufacture
Motherboard layout complete
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="293">
   <si>
     <t>Designator</t>
   </si>
@@ -786,9 +786,6 @@
     <t>22uF</t>
   </si>
   <si>
-    <t>100uF</t>
-  </si>
-  <si>
     <t>4k3</t>
   </si>
   <si>
@@ -835,9 +832,6 @@
   </si>
   <si>
     <t>0.05R 1W 1206 1%</t>
-  </si>
-  <si>
-    <t>http://uk.farnell.com/panasonic-electronic-components/eca2am101/cap-alu-elec-100uf-100v-rad/dp/9693947?st=ECA-2AM101</t>
   </si>
   <si>
     <t xml:space="preserve">MCRH50V226M5X11 </t>
@@ -1268,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,25 +1372,25 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8">
+      <c r="B8" s="4">
         <v>34162</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>176</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9">
+      <c r="B9" s="4">
         <v>165035</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>176</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1414,715 +1408,710 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
-        <v>212</v>
-      </c>
       <c r="C11" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>211</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>217</v>
+      <c r="B12" s="4">
+        <v>14825295</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>227</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>225</v>
+      <c r="B13" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>218</v>
+        <v>238</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>223</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>220</v>
+      <c r="B14" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>216</v>
+        <v>235</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>245</v>
+      <c r="B15" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>219</v>
+        <v>133</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>226</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>224</v>
+      <c r="B16" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>221</v>
+        <v>156</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="5"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="4">
-        <v>14825295</v>
-      </c>
-      <c r="C18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>238</v>
+        <v>247</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="4">
+        <v>61400416121</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
         <v>118</v>
       </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E26">
-        <v>4</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="E29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>204</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
       </c>
       <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>243</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
       </c>
       <c r="E31">
-        <v>8</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F32" s="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="4">
-        <v>61400416121</v>
+        <v>111</v>
+      </c>
+      <c r="B33" t="s">
+        <v>138</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="E33">
         <v>1</v>
-      </c>
-      <c r="F33" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>110</v>
-      </c>
       <c r="B35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" t="s">
-        <v>118</v>
+        <v>160</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
+      <c r="F35" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
+      <c r="F37" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>118</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>109</v>
-      </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E40">
-        <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>159</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>160</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>157</v>
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>263</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>261</v>
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>262</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>249</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>115</v>
-      </c>
       <c r="B44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>52</v>
+        <v>250</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>142</v>
-      </c>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F49" t="s">
-        <v>105</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>106</v>
-      </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>234</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" t="s">
-        <v>71</v>
+        <v>170</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="E52">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F53" s="3"/>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>23</v>
-      </c>
       <c r="B54" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" t="s">
-        <v>25</v>
+        <v>270</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="E54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>58</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>61</v>
+      <c r="F55" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="E56">
-        <v>5</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>170</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>169</v>
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" t="s">
-        <v>66</v>
+      <c r="B58" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="E58">
-        <v>3</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>67</v>
+        <v>2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" t="s">
-        <v>41</v>
+      <c r="A59" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" t="s">
-        <v>38</v>
+      <c r="B60" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="E60">
         <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>37</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C62" t="s">
-        <v>19</v>
+      <c r="B62" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="E62">
         <v>2</v>
       </c>
-      <c r="F62" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>165</v>
-      </c>
-      <c r="B63" t="s">
-        <v>162</v>
+      <c r="B63" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" t="s">
-        <v>68</v>
+      <c r="B64" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="E64">
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
-        <v>173</v>
+      <c r="B65" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>166</v>
+        <v>97</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" t="s">
-        <v>97</v>
+      <c r="B66" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="E66">
         <v>2</v>
       </c>
-      <c r="F66" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
+      <c r="B67" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E67">
@@ -2130,10 +2119,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
+      <c r="B68" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E68">
@@ -2141,10 +2130,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+      <c r="B69" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E69">
@@ -2152,7 +2141,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+      <c r="B70" s="7" t="s">
         <v>174</v>
       </c>
       <c r="C70" s="7" t="s">
@@ -2166,191 +2155,121 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>15</v>
-      </c>
-      <c r="B71" t="s">
-        <v>124</v>
-      </c>
-      <c r="C71" t="s">
-        <v>21</v>
+      <c r="B71" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>254</v>
       </c>
       <c r="E71">
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>16</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E73">
+      <c r="E74">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E75">
+      <c r="E76">
         <v>2</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>249</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>252</v>
+      <c r="B77" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
-        <v>250</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>268</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F79" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>264</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
-        <v>265</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
-        <v>266</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>278</v>
-      </c>
-      <c r="C83" s="5" t="s">
+      <c r="B78" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>267</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B85" t="s">
-        <v>279</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>272</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E86">
+      <c r="E78">
         <v>2</v>
-      </c>
-      <c r="F86" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
-        <v>40</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E87">
-        <v>6</v>
-      </c>
-      <c r="F87" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F75" r:id="rId1" display="https://www.digikey.co.uk/product-detail/en/rohm-semiconductor/KTR18EZPF2202/RHM22.0KAITR-ND/1983713"/>
-    <hyperlink ref="F55" r:id="rId2"/>
-    <hyperlink ref="F56" r:id="rId3"/>
-    <hyperlink ref="F58" r:id="rId4"/>
-    <hyperlink ref="F44" r:id="rId5"/>
+    <hyperlink ref="F76" r:id="rId1" display="https://www.digikey.co.uk/product-detail/en/rohm-semiconductor/KTR18EZPF2202/RHM22.0KAITR-ND/1983713"/>
+    <hyperlink ref="F50" r:id="rId2"/>
+    <hyperlink ref="F51" r:id="rId3"/>
+    <hyperlink ref="F53" r:id="rId4"/>
+    <hyperlink ref="F37" r:id="rId5"/>
     <hyperlink ref="F2" r:id="rId6"/>
-    <hyperlink ref="F35" r:id="rId7"/>
-    <hyperlink ref="F46" r:id="rId8"/>
-    <hyperlink ref="F21" r:id="rId9"/>
-    <hyperlink ref="F18" r:id="rId10"/>
-    <hyperlink ref="F23" r:id="rId11"/>
-    <hyperlink ref="F30" r:id="rId12"/>
+    <hyperlink ref="F29" r:id="rId7"/>
+    <hyperlink ref="F39" r:id="rId8"/>
+    <hyperlink ref="F15" r:id="rId9"/>
+    <hyperlink ref="F12" r:id="rId10"/>
+    <hyperlink ref="F17" r:id="rId11"/>
+    <hyperlink ref="F24" r:id="rId12"/>
     <hyperlink ref="F6" r:id="rId13"/>
-    <hyperlink ref="F22" r:id="rId14"/>
-    <hyperlink ref="F19" r:id="rId15"/>
-    <hyperlink ref="F51" r:id="rId16"/>
-    <hyperlink ref="F29" r:id="rId17"/>
+    <hyperlink ref="F16" r:id="rId14"/>
+    <hyperlink ref="F13" r:id="rId15"/>
+    <hyperlink ref="F46" r:id="rId16"/>
+    <hyperlink ref="F23" r:id="rId17"/>
     <hyperlink ref="F4" r:id="rId18"/>
     <hyperlink ref="F7" r:id="rId19"/>
   </hyperlinks>
@@ -2361,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,72 +2351,127 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>292</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2507,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2783,6 +2757,34 @@
       </c>
       <c r="E20">
         <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PRSBB & corrections
Added PRS10 breakout board and numerous corrections to footprints
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -4,15 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20172" windowHeight="7716"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20172" windowHeight="7716" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Misc_kit" sheetId="4" r:id="rId2"/>
-    <sheet name="Considered" sheetId="2" r:id="rId3"/>
-    <sheet name="RS232" sheetId="3" r:id="rId4"/>
+    <sheet name="PRS10" sheetId="1" r:id="rId1"/>
+    <sheet name="Awaiting" sheetId="5" r:id="rId2"/>
+    <sheet name="Misc_kit" sheetId="4" r:id="rId3"/>
+    <sheet name="Considered" sheetId="2" r:id="rId4"/>
+    <sheet name="RS232" sheetId="3" r:id="rId5"/>
+    <sheet name="PRSBB" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="311">
   <si>
     <t>Designator</t>
   </si>
@@ -901,6 +904,60 @@
   </si>
   <si>
     <t>553-0700-01</t>
+  </si>
+  <si>
+    <t>LM338K</t>
+  </si>
+  <si>
+    <t>TO-3 voltage regulator</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>1251190P</t>
+  </si>
+  <si>
+    <t>CRG1206 SMT Chip Resistor 1K 0.25W</t>
+  </si>
+  <si>
+    <t>Onecall</t>
+  </si>
+  <si>
+    <t>CAP, MLCC, X7R, 4.7UF, 50V, 1206</t>
+  </si>
+  <si>
+    <t>100uF caps</t>
+  </si>
+  <si>
+    <t>Fastpack</t>
+  </si>
+  <si>
+    <t>2k resistors?</t>
+  </si>
+  <si>
+    <t>PCB mounting SMA connector</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/sma-connectors/7839638/</t>
+  </si>
+  <si>
+    <t>SMA-CONNECTOR</t>
+  </si>
+  <si>
+    <t>MCWR12X1001FTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMK316BJ475KL-T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ8ENF2001V </t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1545,6 +1602,9 @@
       <c r="C21" s="7" t="s">
         <v>189</v>
       </c>
+      <c r="D21" t="s">
+        <v>303</v>
+      </c>
       <c r="E21">
         <v>4</v>
       </c>
@@ -1844,217 +1904,217 @@
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>293</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>106</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>34</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>35</v>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3" t="s">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
         <v>72</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>71</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <v>6</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F48" s="3"/>
-    </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>23</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>119</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>25</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>4</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>170</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>168</v>
+        <v>62</v>
+      </c>
+      <c r="C52" t="s">
+        <v>63</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" t="s">
-        <v>66</v>
+        <v>170</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>270</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>253</v>
+        <v>65</v>
+      </c>
+      <c r="C54" t="s">
+        <v>66</v>
       </c>
       <c r="E54">
-        <v>2</v>
-      </c>
-      <c r="F54" t="s">
-        <v>271</v>
+        <v>3</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C55" t="s">
-        <v>41</v>
+        <v>270</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>39</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
         <v>36</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>38</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <v>2</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="7" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E58">
+      <c r="E59">
         <v>2</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>165</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E60">
-        <v>2</v>
-      </c>
-      <c r="F60" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="E61">
         <v>2</v>
       </c>
+      <c r="F61" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
-        <v>128</v>
+        <v>263</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -2062,68 +2122,68 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="7" t="s">
-        <v>264</v>
+        <v>173</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>257</v>
+        <v>166</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B65" s="7" t="s">
-        <v>126</v>
+        <v>264</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>97</v>
+        <v>257</v>
       </c>
       <c r="E65">
         <v>2</v>
       </c>
-      <c r="F65" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B66" s="7" t="s">
-        <v>265</v>
+        <v>126</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>256</v>
+        <v>97</v>
       </c>
       <c r="E66">
         <v>2</v>
       </c>
+      <c r="F66" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B67" s="7" t="s">
-        <v>120</v>
+        <v>265</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>99</v>
+        <v>256</v>
       </c>
       <c r="E67">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E68">
         <v>3</v>
@@ -2131,132 +2191,143 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B69" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B70" s="7" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70" t="s">
-        <v>175</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B71" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>15</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="E72">
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>15</v>
+      </c>
       <c r="B73" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C74" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B75" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C75" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B75" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E75">
-        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="E76">
-        <v>2</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B77" s="7" t="s">
-        <v>266</v>
+        <v>122</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>259</v>
+        <v>22</v>
       </c>
       <c r="E77">
         <v>2</v>
       </c>
+      <c r="F77" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B78" s="7" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E78">
         <v>2</v>
       </c>
     </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F76" r:id="rId1" display="https://www.digikey.co.uk/product-detail/en/rohm-semiconductor/KTR18EZPF2202/RHM22.0KAITR-ND/1983713"/>
-    <hyperlink ref="F50" r:id="rId2"/>
-    <hyperlink ref="F51" r:id="rId3"/>
-    <hyperlink ref="F53" r:id="rId4"/>
+    <hyperlink ref="F77" r:id="rId1" display="https://www.digikey.co.uk/product-detail/en/rohm-semiconductor/KTR18EZPF2202/RHM22.0KAITR-ND/1983713"/>
+    <hyperlink ref="F51" r:id="rId2"/>
+    <hyperlink ref="F52" r:id="rId3"/>
+    <hyperlink ref="F54" r:id="rId4"/>
     <hyperlink ref="F37" r:id="rId5"/>
     <hyperlink ref="F2" r:id="rId6"/>
     <hyperlink ref="F29" r:id="rId7"/>
@@ -2268,7 +2339,7 @@
     <hyperlink ref="F6" r:id="rId13"/>
     <hyperlink ref="F16" r:id="rId14"/>
     <hyperlink ref="F13" r:id="rId15"/>
-    <hyperlink ref="F46" r:id="rId16"/>
+    <hyperlink ref="F47" r:id="rId16"/>
     <hyperlink ref="F23" r:id="rId17"/>
     <hyperlink ref="F4" r:id="rId18"/>
     <hyperlink ref="F7" r:id="rId19"/>
@@ -2279,6 +2350,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>419001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>419002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>2320908</v>
+      </c>
+      <c r="E3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>419116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -2479,7 +2631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -2795,7 +2947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2869,4 +3021,313 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="43.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="4">
+        <v>61400416121</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F16" r:id="rId1"/>
+    <hyperlink ref="F17" r:id="rId2"/>
+    <hyperlink ref="F18" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="F13" r:id="rId5"/>
+    <hyperlink ref="F12" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Front panel outline & cutouts
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20172" windowHeight="7716"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20175" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="PRS10" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="PRSBB" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1327,21 +1326,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1375,10 +1374,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>94</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>143</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>229</v>
       </c>
@@ -1420,7 +1419,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>208</v>
       </c>
@@ -1434,7 +1433,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>34162</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>165035</v>
       </c>
@@ -1456,7 +1455,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>179</v>
       </c>
@@ -1470,12 +1469,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>14825295</v>
       </c>
@@ -1489,7 +1488,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>149</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>237</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>135</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>181</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>131</v>
       </c>
@@ -1562,7 +1561,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>197</v>
       </c>
@@ -1573,7 +1572,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>247</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>232</v>
       </c>
@@ -1601,7 +1600,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>195</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>200</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>203</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>206</v>
       </c>
@@ -1660,7 +1659,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>242</v>
       </c>
@@ -1674,10 +1673,10 @@
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -1690,11 +1689,11 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -1759,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>111</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>160</v>
       </c>
@@ -1818,7 +1817,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>85</v>
       </c>
@@ -1866,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>49</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>103</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>249</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>250</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>293</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>311</v>
       </c>
@@ -1932,7 +1931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>72</v>
       </c>
@@ -1963,10 +1962,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>59</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>62</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>170</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>65</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>270</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>40</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>36</v>
       </c>
@@ -2081,7 +2080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
         <v>274</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>165</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
         <v>267</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="7" t="s">
         <v>263</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="7" t="s">
         <v>128</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
         <v>173</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="s">
         <v>264</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
         <v>126</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="s">
         <v>265</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="s">
         <v>120</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
         <v>127</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="s">
         <v>123</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="s">
         <v>174</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" s="7" t="s">
         <v>276</v>
       </c>
@@ -2253,7 +2252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
         <v>125</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="7" t="s">
         <v>121</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="s">
         <v>122</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
         <v>266</v>
       </c>
@@ -2328,7 +2327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
         <v>277</v>
       </c>
@@ -2360,9 +2359,11 @@
     <hyperlink ref="F23" r:id="rId17"/>
     <hyperlink ref="F4" r:id="rId18"/>
     <hyperlink ref="F7" r:id="rId19"/>
+    <hyperlink ref="F27" r:id="rId20"/>
+    <hyperlink ref="F19" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -2374,13 +2375,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>295</v>
       </c>
@@ -2394,7 +2395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>419001</v>
       </c>
@@ -2408,7 +2409,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>419002</v>
       </c>
@@ -2422,7 +2423,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>419116</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>310</v>
       </c>
@@ -2455,14 +2456,14 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4">
         <v>430019</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>231</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>241</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>278</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>283</v>
       </c>
@@ -2546,7 +2547,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>286</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>289</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>292</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>246</v>
       </c>
@@ -2599,7 +2600,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>225</v>
       </c>
@@ -2610,7 +2611,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>220</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>245</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>224</v>
       </c>
@@ -2656,15 +2657,15 @@
       <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>45</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>74</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2792,7 +2793,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -2832,7 +2833,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -2849,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -2866,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>191</v>
       </c>
@@ -2900,13 +2901,13 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C18" s="5" t="s">
         <v>150</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>213</v>
       </c>
@@ -2914,7 +2915,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>212</v>
       </c>
@@ -2942,7 +2943,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>262</v>
       </c>
@@ -2972,14 +2973,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2996,7 +2997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>121</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>182</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>185</v>
       </c>
@@ -3048,17 +3049,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>307</v>
       </c>
@@ -3089,8 +3090,8 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -3107,8 +3108,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>85</v>
       </c>
@@ -3119,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -3133,8 +3134,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>72</v>
       </c>
@@ -3148,8 +3149,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -3186,7 +3187,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -3206,8 +3207,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3224,7 +3225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>59</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>62</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>309</v>
       </c>
@@ -3266,7 +3267,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>128</v>
       </c>
@@ -3277,7 +3278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>126</v>
       </c>
@@ -3291,7 +3292,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>308</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>127</v>
       </c>
@@ -3313,7 +3314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>125</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>121</v>
       </c>

</xml_diff>